<commit_message>
PROS-5087 Zodac brand block KPI correction
I updated the template - brand blocking sheet.
</commit_message>
<xml_diff>
--- a/Projects/SANOFIRU/Data/Template.xlsx
+++ b/Projects/SANOFIRU/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$31</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
@@ -43,6 +43,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
@@ -65,6 +66,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Primary_Brand_Blocking!$A$2:$H$12</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
@@ -75,29 +77,30 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$31</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$J$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$J$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$31</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$31</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$J$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$J$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -111,474 +114,474 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="141">
   <si>
-    <t>KPI Name</t>
+    <t xml:space="preserve">KPI Name</t>
   </si>
   <si>
-    <t>KPI Group</t>
+    <t xml:space="preserve">KPI Group</t>
   </si>
   <si>
-    <t>KPI Type</t>
+    <t xml:space="preserve">KPI Type</t>
   </si>
   <si>
-    <t>Tested Group</t>
+    <t xml:space="preserve">Tested Group</t>
   </si>
   <si>
-    <t>Template Group</t>
+    <t xml:space="preserve">Template Group</t>
   </si>
   <si>
-    <t>Sheet</t>
+    <t xml:space="preserve">Sheet</t>
   </si>
   <si>
-    <t>SCORE</t>
+    <t xml:space="preserve">SCORE</t>
   </si>
   <si>
-    <t>POSM Availability Primary</t>
+    <t xml:space="preserve">POSM Availability Primary</t>
   </si>
   <si>
-    <t>Primary Shelf</t>
+    <t xml:space="preserve">Primary Shelf</t>
   </si>
   <si>
-    <t>Product Availability Per SKU</t>
+    <t xml:space="preserve">Product Availability Per SKU</t>
   </si>
   <si>
-    <t>Primary&amp;Secondary_POSM</t>
+    <t xml:space="preserve">Primary&amp;Secondary_POSM</t>
   </si>
   <si>
-    <t>numeric</t>
+    <t xml:space="preserve">numeric</t>
   </si>
   <si>
-    <t>Product Minimum Facings Primary</t>
+    <t xml:space="preserve">Product Minimum Facings Primary</t>
   </si>
   <si>
-    <t>Primary&amp;Secondary_Facings</t>
+    <t xml:space="preserve">Primary&amp;Secondary_Facings</t>
   </si>
   <si>
-    <t>Blocked Together</t>
+    <t xml:space="preserve">Blocked Together</t>
   </si>
   <si>
-    <t>Blocked Together Per Brand</t>
+    <t xml:space="preserve">Blocked Together Per Brand</t>
   </si>
   <si>
-    <t>Primary_Brand_Blocking</t>
+    <t xml:space="preserve">Primary_Brand_Blocking</t>
   </si>
   <si>
-    <t>POSM Availability Secondary</t>
+    <t xml:space="preserve">POSM Availability Secondary</t>
   </si>
   <si>
-    <t>Secondary Shelf</t>
+    <t xml:space="preserve">Secondary Shelf</t>
   </si>
   <si>
-    <t>Product Minimum Facings Secondary</t>
+    <t xml:space="preserve">Product Minimum Facings Secondary</t>
   </si>
   <si>
-    <t>MSL Compliance</t>
+    <t xml:space="preserve">MSL Compliance</t>
   </si>
   <si>
-    <t>MSL</t>
+    <t xml:space="preserve">MSL</t>
   </si>
   <si>
-    <t>Perfect Store</t>
+    <t xml:space="preserve">Perfect Store</t>
   </si>
   <si>
-    <t>Primary Shelf Compliance</t>
+    <t xml:space="preserve">Primary Shelf Compliance</t>
   </si>
   <si>
-    <t>Secondary Shelf Compliance</t>
+    <t xml:space="preserve">Secondary Shelf Compliance</t>
   </si>
   <si>
-    <t>Perfect Store Compliance</t>
+    <t xml:space="preserve">Perfect Store Compliance</t>
   </si>
   <si>
-    <t>Sum of KPIs in Group</t>
+    <t xml:space="preserve">Sum of KPIs in Group</t>
   </si>
   <si>
-    <t>store type</t>
+    <t xml:space="preserve">store type</t>
   </si>
   <si>
-    <t>Product Name</t>
+    <t xml:space="preserve">Product Name</t>
   </si>
   <si>
-    <t>Product EAN Code</t>
+    <t xml:space="preserve">Product EAN Code</t>
   </si>
   <si>
-    <t>Brand</t>
+    <t xml:space="preserve">Brand</t>
   </si>
   <si>
-    <t>Category</t>
+    <t xml:space="preserve">Category</t>
   </si>
   <si>
-    <t>Points</t>
+    <t xml:space="preserve">Points</t>
   </si>
   <si>
-    <t>A w/ POSM w/ CD</t>
+    <t xml:space="preserve">A w/ POSM w/ CD</t>
   </si>
   <si>
-    <t>A w/ POSM w/o CD</t>
+    <t xml:space="preserve">A w/ POSM w/o CD</t>
   </si>
   <si>
-    <t>A w/o POSM w/ CD</t>
+    <t xml:space="preserve">A w/o POSM w/ CD</t>
   </si>
   <si>
-    <t>A w/o POSM w/o CD</t>
+    <t xml:space="preserve">A w/o POSM w/o CD</t>
   </si>
   <si>
-    <t>B-1 w/ POSM w/ CD</t>
+    <t xml:space="preserve">B-1 w/ POSM w/ CD</t>
   </si>
   <si>
-    <t>B-1 w/ POSM w/o CD</t>
+    <t xml:space="preserve">B-1 w/ POSM w/o CD</t>
   </si>
   <si>
-    <t>B-1 w/o POSM w/ CD</t>
+    <t xml:space="preserve">B-1 w/o POSM w/ CD</t>
   </si>
   <si>
-    <t>B-1 w/o POSM w/o CD</t>
+    <t xml:space="preserve">B-1 w/o POSM w/o CD</t>
   </si>
   <si>
-    <t>B-2 w/ POSM w/ CD</t>
+    <t xml:space="preserve">B-2 w/ POSM w/ CD</t>
   </si>
   <si>
-    <t>B-2 w/ POSM w/o CD</t>
+    <t xml:space="preserve">B-2 w/ POSM w/o CD</t>
   </si>
   <si>
-    <t>B-2 w/o POSM w/ CD</t>
+    <t xml:space="preserve">B-2 w/o POSM w/ CD</t>
   </si>
   <si>
-    <t>B-2 w/o POSM w/o CD</t>
+    <t xml:space="preserve">B-2 w/o POSM w/o CD</t>
   </si>
   <si>
-    <t>B-3 w/ POSM w/ CD</t>
+    <t xml:space="preserve">B-3 w/ POSM w/ CD</t>
   </si>
   <si>
-    <t>B-3 w/ POSM w/o CD</t>
+    <t xml:space="preserve">B-3 w/ POSM w/o CD</t>
   </si>
   <si>
-    <t>B-3 w/o POSM w/ CD</t>
+    <t xml:space="preserve">B-3 w/o POSM w/ CD</t>
   </si>
   <si>
-    <t>B-3 w/o POSM w/o CD</t>
+    <t xml:space="preserve">B-3 w/o POSM w/o CD</t>
   </si>
   <si>
-    <t>B-4 w/o POSM w/o CD</t>
+    <t xml:space="preserve">B-4 w/o POSM w/o CD</t>
   </si>
   <si>
-    <t>B-4 w/o POSM w/ CD</t>
+    <t xml:space="preserve">B-4 w/o POSM w/ CD</t>
   </si>
   <si>
-    <t>ESSENTIALE FORTE N 300MG CAP BL9X10</t>
+    <t xml:space="preserve">ESSENTIALE FORTE N 300MG CAP BL9X10</t>
   </si>
   <si>
-    <t>ESSENTIALE</t>
+    <t xml:space="preserve">ESSENTIALE</t>
   </si>
   <si>
-    <t>Hepatoprotectors</t>
+    <t xml:space="preserve">Hepatoprotectors</t>
   </si>
   <si>
-    <t>ESSENTIALE FORTE N CAPS 300MG #30</t>
+    <t xml:space="preserve">ESSENTIALE FORTE N CAPS 300MG #30</t>
   </si>
   <si>
-    <t>FESTAL DRAGEE 200MG #20</t>
+    <t xml:space="preserve">FESTAL DRAGEE 200MG #20</t>
   </si>
   <si>
-    <t>FESTAL</t>
+    <t xml:space="preserve">FESTAL</t>
   </si>
   <si>
-    <t>DH</t>
+    <t xml:space="preserve">DH</t>
   </si>
   <si>
-    <t>FESTAL DRAGEE 200MG #40</t>
+    <t xml:space="preserve">FESTAL DRAGEE 200MG #40</t>
   </si>
   <si>
-    <t>FESTAL DRAGEE 200MG #100</t>
+    <t xml:space="preserve">FESTAL DRAGEE 200MG #100</t>
   </si>
   <si>
-    <t>MAALOX TABS 400MG #20</t>
+    <t xml:space="preserve">MAALOX TABS 400MG #20</t>
   </si>
   <si>
-    <t>MAALOX</t>
+    <t xml:space="preserve">MAALOX</t>
   </si>
   <si>
-    <t>MAALOX stick pack 4,3ml #6 red fruit taste</t>
+    <t xml:space="preserve">MAALOX stick pack 4,3ml #6 red fruit taste</t>
   </si>
   <si>
-    <t>GUTTALAX 300MG/40ML 30ML EEDRO BT1 M36RU</t>
+    <t xml:space="preserve">GUTTALAX 300MG/40ML 30ML EEDRO BT1 M36RU</t>
   </si>
   <si>
-    <t>GUTTALAX</t>
+    <t xml:space="preserve">GUTTALAX</t>
   </si>
   <si>
-    <t>LASOLVAN 300MG/40ML SOLIN BT1 M60 RU</t>
+    <t xml:space="preserve">LASOLVAN 300MG/40ML SOLIN BT1 M60 RU</t>
   </si>
   <si>
-    <t>LASOLVAN</t>
+    <t xml:space="preserve">LASOLVAN</t>
   </si>
   <si>
-    <t>C&amp;C</t>
+    <t xml:space="preserve">C&amp;C</t>
   </si>
   <si>
-    <t>LASOLVAN 15mg/5ml Syrup 100ml</t>
+    <t xml:space="preserve">LASOLVAN 15mg/5ml Syrup 100ml</t>
   </si>
   <si>
-    <t>LASOLVAN 30mg/5ml Syrup 100ml</t>
+    <t xml:space="preserve">LASOLVAN 30mg/5ml Syrup 100ml</t>
   </si>
   <si>
-    <t>LASOLVAN MAX 75MG CAPCR BL1X10 M36 RU</t>
+    <t xml:space="preserve">LASOLVAN MAX 75MG CAPCR BL1X10 M36 RU</t>
   </si>
   <si>
-    <t>MAGNE B6 TABS 48MG/5MG BLIST #50</t>
+    <t xml:space="preserve">MAGNE B6 TABS 48MG/5MG BLIST #50</t>
   </si>
   <si>
-    <t>MAGNE B6</t>
+    <t xml:space="preserve">MAGNE B6</t>
   </si>
   <si>
-    <t>VMS</t>
+    <t xml:space="preserve">VMS</t>
   </si>
   <si>
-    <t>MAGNE B6 AMP 100MG/ 10MG/ 10ML #10</t>
+    <t xml:space="preserve">MAGNE B6 AMP 100MG/ 10MG/ 10ML #10</t>
   </si>
   <si>
-    <t>MAGNE B6 FORTE #30</t>
+    <t xml:space="preserve">MAGNE B6 FORTE #30</t>
   </si>
   <si>
-    <t>D-SUN LEMON 20ML DROP</t>
+    <t xml:space="preserve">D-SUN LEMON 20ML DROP</t>
   </si>
   <si>
-    <t>D-Sun</t>
+    <t xml:space="preserve">D-Sun</t>
   </si>
   <si>
-    <t>D-SUN RASPBERRY 10ML DROP</t>
+    <t xml:space="preserve">D-SUN RASPBERRY 10ML DROP</t>
   </si>
   <si>
-    <t>NO-SPA TABS 40MG #100</t>
+    <t xml:space="preserve">NO-SPA TABS 40MG #100</t>
   </si>
   <si>
-    <t>NO-SPA</t>
+    <t xml:space="preserve">NO-SPA</t>
   </si>
   <si>
-    <t>Pain</t>
+    <t xml:space="preserve">Pain</t>
   </si>
   <si>
-    <t>NO-SPA 40mg #24</t>
+    <t xml:space="preserve">NO-SPA 40mg #24</t>
   </si>
   <si>
-    <t>NO-SPA TAB 40 MG (PUSH-TOP) #60</t>
+    <t xml:space="preserve">NO-SPA TAB 40 MG (PUSH-TOP) #60</t>
   </si>
   <si>
-    <t>NO-SPA FORTE 80MG TAB BL1X24 M36 RU</t>
+    <t xml:space="preserve">NO-SPA FORTE 80MG TAB BL1X24 M36 RU</t>
   </si>
   <si>
-    <t>FINALGON CREAM/35G 1/1,7+10,8MG/G RUS</t>
+    <t xml:space="preserve">FINALGON CREAM/35G 1/1,7+10,8MG/G RUS</t>
   </si>
   <si>
-    <t>
+    <t xml:space="preserve">
 3582910082682 </t>
   </si>
   <si>
-    <t>FINALGON</t>
+    <t xml:space="preserve">FINALGON</t>
   </si>
   <si>
-    <t>FINALGON 25MG-4MG/G OINT TB1 M48 RU</t>
+    <t xml:space="preserve">FINALGON 25MG-4MG/G OINT TB1 M48 RU</t>
   </si>
   <si>
-    <t>Zodac GTT.20ML</t>
+    <t xml:space="preserve">Zodac GTT.20ML</t>
   </si>
   <si>
-    <t>ZODAC</t>
+    <t xml:space="preserve">ZODAC</t>
   </si>
   <si>
-    <t>Allergy</t>
+    <t xml:space="preserve">Allergy</t>
   </si>
   <si>
-    <t>Zodac TABS.FLM.30X10MG</t>
+    <t xml:space="preserve">Zodac TABS.FLM.30X10MG</t>
   </si>
   <si>
-    <t>SKUs</t>
+    <t xml:space="preserve">SKUs</t>
   </si>
   <si>
-    <t>Shelf Location Compliance</t>
+    <t xml:space="preserve">Shelf Location Compliance</t>
   </si>
   <si>
-    <t>Ignore Empty</t>
+    <t xml:space="preserve">Ignore Empty</t>
   </si>
   <si>
-    <t>ESSENTIALE FORTE N 300MG CAP BL9X10,
+    <t xml:space="preserve">ESSENTIALE FORTE N 300MG CAP BL9X10,
 ESSENTIALE FORTE N CAPS 300MG #30</t>
   </si>
   <si>
-    <t>3582910078913,
+    <t xml:space="preserve">3582910078913,
 3582910077305</t>
   </si>
   <si>
-    <t>FESTAL DRAGEE 200MG #20,
+    <t xml:space="preserve">FESTAL DRAGEE 200MG #20,
 FESTAL DRAGEE 200MG #40,
 FESTAL DRAGEE 200MG #100</t>
   </si>
   <si>
-    <t>8901083060122,
+    <t xml:space="preserve">8901083060122,
 8901083060139,
 8901083060115</t>
   </si>
   <si>
-    <t>FESTAL DRAGEE 200MG #20,
+    <t xml:space="preserve">FESTAL DRAGEE 200MG #20,
 FESTAL DRAGEE 200MG #40</t>
   </si>
   <si>
-    <t>8901083060122,
+    <t xml:space="preserve">8901083060122,
 8901083060139</t>
   </si>
   <si>
-    <t>MAALOX TABS 400MG #20,
+    <t xml:space="preserve">MAALOX TABS 400MG #20,
 MAALOX stick pack 4,3ml #6 red fruit taste</t>
   </si>
   <si>
-    <t>3582910072218,
+    <t xml:space="preserve">3582910072218,
 3582910075660</t>
   </si>
   <si>
-    <t>Guttalax</t>
+    <t xml:space="preserve">Guttalax</t>
   </si>
   <si>
-    <t>LASOLVAN 300MG/40ML SOLIN BT1 M60 RU, 
+    <t xml:space="preserve">LASOLVAN 300MG/40ML SOLIN BT1 M60 RU, 
 LASOLVAN 15mg/5ml Syrup 100ml,
 LASOLVAN 30mg/5ml Syrup 100ml,
 LASOLVAN MAX 75MG CAPCR BL1X10 M36 RU,</t>
   </si>
   <si>
-    <t>9006968004082,
+    <t xml:space="preserve">9006968004082,
 9006968011882,
 9006968011479,
 9006968010793</t>
   </si>
   <si>
-    <t>LASOLVAN 300MG/40ML SOLIN BT1 M60 RU, 
+    <t xml:space="preserve">LASOLVAN 300MG/40ML SOLIN BT1 M60 RU, 
 LASOLVAN 15mg/5ml Syrup 100ml,
 LASOLVAN 30mg/5ml Syrup 100ml</t>
   </si>
   <si>
-    <t>9006968004082,
+    <t xml:space="preserve">9006968004082,
 9006968011882,
 9006968011479</t>
   </si>
   <si>
-    <t>MAGNE B6 TABS 48MG/5MG BLIST #50,
+    <t xml:space="preserve">MAGNE B6 TABS 48MG/5MG BLIST #50,
 MAGNE B6 AMP 100MG/ 10MG/ 10ML #10,
 MAGNE B6 FORTE #30</t>
   </si>
   <si>
-    <t>3582910070252,
+    <t xml:space="preserve">3582910070252,
 3582910026723,
 3582910071259</t>
   </si>
   <si>
-    <t>MAGNE B6 TABS 48MG/5MG BLIST #50,
+    <t xml:space="preserve">MAGNE B6 TABS 48MG/5MG BLIST #50,
 MAGNE B6 FORTE #30</t>
   </si>
   <si>
-    <t>3582910070252,
+    <t xml:space="preserve">3582910070252,
 3582910071259</t>
   </si>
   <si>
-    <t>D-SUN LEMON 20ML DROP,
+    <t xml:space="preserve">D-SUN LEMON 20ML DROP,
 D-SUN RASPBERRY 10ML DROP</t>
   </si>
   <si>
-    <t>7896070607590,
+    <t xml:space="preserve">7896070607590,
 7896070607606</t>
   </si>
   <si>
-    <t>NO-SPA TABS 40MG #100,
+    <t xml:space="preserve">NO-SPA TABS 40MG #100,
 NO-SPA 40mg #24,
 NO-SPA TAB 40 MG (PUSH-TOP) #60,
 NO-SPA FORTE 80MG TAB BL1X24 M36 RU</t>
   </si>
   <si>
-    <t>5997086103280,
+    <t xml:space="preserve">5997086103280,
 3582910060758,
 5997086105055,
 3582910062172</t>
   </si>
   <si>
-    <t>NO-SPA TABS 40MG #100,
+    <t xml:space="preserve">NO-SPA TABS 40MG #100,
 NO-SPA 40mg #24,
 NO-SPA TAB 40 MG (PUSH-TOP) #60</t>
   </si>
   <si>
-    <t>5997086103280,
+    <t xml:space="preserve">5997086103280,
 3582910060758,
 5997086105055</t>
   </si>
   <si>
-    <t>NO-SPA TABS 40MG #100,
+    <t xml:space="preserve">NO-SPA TABS 40MG #100,
 NO-SPA 40mg #24</t>
   </si>
   <si>
-    <t>5997086103280,
+    <t xml:space="preserve">5997086103280,
 3582910060758</t>
   </si>
   <si>
-    <t>FINALGON CREAM/35G 1/1,7+10,8MG/G RUS,
+    <t xml:space="preserve">FINALGON CREAM/35G 1/1,7+10,8MG/G RUS,
 FINALGON 25MG-4MG/G OINT TB1 M48 RU</t>
   </si>
   <si>
-    <t>3582910082682,
+    <t xml:space="preserve">3582910082682,
 9006968004532</t>
   </si>
   <si>
-    <t>Zodac TABS.FLM.30X10MG,
+    <t xml:space="preserve">Zodac TABS.FLM.30X10MG,
 Zodac GTT.20ML</t>
   </si>
   <si>
-    <t>8594739055421,
+    <t xml:space="preserve">8594739055421,
 8594739055209
 </t>
   </si>
   <si>
-    <t>8594739055209
+    <t xml:space="preserve">8594739055209
 </t>
   </si>
   <si>
-    <t>D-Sun primary POSM</t>
+    <t xml:space="preserve">D-Sun primary POSM</t>
   </si>
   <si>
-    <t>RU-ST-01</t>
+    <t xml:space="preserve">RU-ST-01</t>
   </si>
   <si>
-    <t>Essentiale primary POSM</t>
+    <t xml:space="preserve">Essentiale primary POSM</t>
   </si>
   <si>
-    <t>RU-ST-02</t>
+    <t xml:space="preserve">RU-ST-02</t>
   </si>
   <si>
-    <t>Essentiale</t>
+    <t xml:space="preserve">Essentiale</t>
   </si>
   <si>
-    <t>Lasolvan primary POSM</t>
+    <t xml:space="preserve">Lasolvan primary POSM</t>
   </si>
   <si>
-    <t>RU-ST-03</t>
+    <t xml:space="preserve">RU-ST-03</t>
   </si>
   <si>
-    <t>Lasolvan</t>
+    <t xml:space="preserve">Lasolvan</t>
   </si>
   <si>
-    <t>Magne B6 primary POSM</t>
+    <t xml:space="preserve">Magne B6 primary POSM</t>
   </si>
   <si>
-    <t>RU-ST-04</t>
+    <t xml:space="preserve">RU-ST-04</t>
   </si>
   <si>
-    <t>Magne B6</t>
+    <t xml:space="preserve">Magne B6</t>
   </si>
   <si>
-    <t>No-spa primary POSM</t>
+    <t xml:space="preserve">No-spa primary POSM</t>
   </si>
   <si>
-    <t>RU-ST-05</t>
+    <t xml:space="preserve">RU-ST-05</t>
   </si>
   <si>
-    <t>No-Spa</t>
+    <t xml:space="preserve">No-Spa</t>
   </si>
   <si>
-    <t>No Spa 40 mg city pack #6</t>
+    <t xml:space="preserve">No Spa 40 mg city pack #6</t>
   </si>
 </sst>
 </file>
@@ -586,12 +589,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -729,6 +732,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1025,7 +1035,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1282,6 +1292,22 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1294,7 +1320,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1346,7 +1372,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="6" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="22" fillId="6" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1392,14 +1418,6 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="13" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1524,7 +1542,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4106880" y="1474920"/>
+          <a:off x="4180680" y="1474920"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1548,7 +1566,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>915480</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>378000</xdr:rowOff>
+      <xdr:rowOff>377640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1561,8 +1579,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4020120" y="1462320"/>
-          <a:ext cx="360" cy="116280"/>
+          <a:off x="4093920" y="1462320"/>
+          <a:ext cx="360" cy="115920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1588,9 +1606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2000880</xdr:colOff>
+      <xdr:colOff>2000520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>474120</xdr:rowOff>
+      <xdr:rowOff>473760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1603,8 +1621,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4180680" y="901440"/>
-          <a:ext cx="1080" cy="189720"/>
+          <a:off x="4231080" y="901440"/>
+          <a:ext cx="720" cy="189360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1630,19 +1648,19 @@
   </sheetPr>
   <dimension ref="A1:G65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.17004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8947368421053"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0931174089069"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.4412955465587"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.9473684210526"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.834008097166"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,21 +1900,21 @@
   </sheetPr>
   <dimension ref="1:27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.3481781376518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.7611336032389"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0364372469636"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7732793522267"/>
     <col collapsed="false" hidden="true" max="6" min="6" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.2267206477733"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3832,20 +3850,19 @@
   </sheetPr>
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0364372469636"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.82995951417"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.7611336032389"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8947368421053"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.97570850202429"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4240,22 +4257,22 @@
   </sheetPr>
   <dimension ref="A1:AMH21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R27" activeCellId="0" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="52" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="52" width="6"/>
-    <col collapsed="false" hidden="false" max="1022" min="9" style="52" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="14.2024291497976"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="10.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="11.0202429149798"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="40.7611336032389"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="23.0161943319838"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="16.7732793522267"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="52" width="6.24291497975709"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="52" width="6.12145748987854"/>
+    <col collapsed="false" hidden="false" max="1022" min="9" style="52" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9610,7 +9627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="27.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="62" t="s">
         <v>14</v>
       </c>
@@ -9626,135 +9643,135 @@
       <c r="E20" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="F20" s="58" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="59" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="I20" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="J20" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="K20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="R20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="S20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="T20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="U20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="V20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="W20" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="X20" s="60" t="n">
+      <c r="F20" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" s="67" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="65" t="s">
+      <c r="D21" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="66" t="s">
+      <c r="E21" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="F21" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="I21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="J21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="K21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="L21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="M21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="N21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="O21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="P21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="R21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="S21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="T21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="U21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="V21" s="69" t="n">
-        <v>1</v>
-      </c>
-      <c r="W21" s="69" t="n">
-        <v>0</v>
-      </c>
-      <c r="X21" s="70" t="n">
+      <c r="F21" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="P21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="R21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="U21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="V21" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="W21" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" s="74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9781,21 +9798,21 @@
   </sheetPr>
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="58.914979757085"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="52" width="6"/>
-    <col collapsed="false" hidden="false" max="1022" min="8" style="52" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="25.0931174089069"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="26.080971659919"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="60.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="10.6558704453441"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="11.0202429149798"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="6.24291497975709"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="52" width="6.12145748987854"/>
+    <col collapsed="false" hidden="false" max="1022" min="8" style="52" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9897,259 +9914,259 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="75"/>
-      <c r="R3" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" s="75"/>
-      <c r="U3" s="75"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="76"/>
+      <c r="F3" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="79"/>
+      <c r="U3" s="79"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="81" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="81" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="78" t="s">
+      <c r="E4" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="76"/>
-      <c r="W4" s="76"/>
+      <c r="F4" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="83"/>
+      <c r="U4" s="83"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="79" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="S5" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" s="75"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="72"/>
-      <c r="W5" s="72"/>
+      <c r="F5" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="76"/>
+      <c r="W5" s="76"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="79" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="O6" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" s="75"/>
-      <c r="Q6" s="75"/>
-      <c r="R6" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="S6" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="T6" s="75"/>
-      <c r="U6" s="75"/>
-      <c r="V6" s="72"/>
-      <c r="W6" s="72"/>
+      <c r="F6" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="76"/>
+      <c r="W6" s="76"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="79" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" s="75"/>
-      <c r="M7" s="75"/>
-      <c r="N7" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="75"/>
-      <c r="R7" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="S7" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" s="75"/>
-      <c r="U7" s="75"/>
-      <c r="V7" s="72"/>
-      <c r="W7" s="72"/>
+      <c r="F7" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" s="79"/>
+      <c r="Q7" s="79"/>
+      <c r="R7" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" s="79"/>
+      <c r="U7" s="79"/>
+      <c r="V7" s="76"/>
+      <c r="W7" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10174,22 +10191,22 @@
   </sheetPr>
   <dimension ref="1:31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O42" activeCellId="0" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="34.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="52" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="52" width="6"/>
-    <col collapsed="false" hidden="false" max="1022" min="9" style="52" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="32.4412955465587"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="34.8906882591093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="14.3238866396761"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="10.5263157894737"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="10.5263157894737"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="52" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="52" width="6.12145748987854"/>
+    <col collapsed="false" hidden="false" max="1022" min="9" style="52" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10199,26 +10216,26 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
       <c r="F1" s="25"/>
-      <c r="G1" s="80" t="s">
+      <c r="G1" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="80"/>
-      <c r="X1" s="80"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
       <c r="Y1" s="0"/>
       <c r="Z1" s="0"/>
       <c r="AA1" s="0"/>
@@ -11219,22 +11236,22 @@
       <c r="AMH1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="48.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="82" t="s">
+      <c r="A2" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="86" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="29" t="s">
@@ -12291,7 +12308,7 @@
       <c r="AMH2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="32" t="s">
@@ -13363,7 +13380,7 @@
       <c r="AMH3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="32" t="s">
@@ -14435,7 +14452,7 @@
       <c r="AMH4" s="0"/>
     </row>
     <row r="5" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="32" t="s">
@@ -14511,7 +14528,7 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="32" t="s">
@@ -14585,7 +14602,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="32" t="s">
@@ -14659,7 +14676,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="32" t="s">
@@ -14733,7 +14750,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="32" t="s">
@@ -14807,7 +14824,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="84" t="s">
+      <c r="A10" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="32" t="s">
@@ -14881,7 +14898,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="32" t="s">
@@ -14955,7 +14972,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="32" t="s">
@@ -15029,7 +15046,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="71" t="s">
+      <c r="A13" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="32" t="s">
@@ -15103,7 +15120,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="71" t="s">
+      <c r="A14" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="32" t="s">
@@ -15177,7 +15194,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="84" t="s">
+      <c r="A15" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -15251,7 +15268,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="84" t="s">
+      <c r="A16" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="32" t="s">
@@ -15325,7 +15342,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="84" t="s">
+      <c r="A17" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="32" t="s">
@@ -15399,7 +15416,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="32" t="s">
@@ -15473,7 +15490,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="32" t="s">
@@ -15547,7 +15564,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="32" t="s">
@@ -15621,7 +15638,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="32" t="s">
@@ -15695,7 +15712,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="71" t="s">
+      <c r="A22" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -15769,13 +15786,13 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="85" t="n">
+      <c r="C23" s="89" t="n">
         <v>3582910062172</v>
       </c>
       <c r="D23" s="34" t="s">
@@ -15843,13 +15860,13 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="86" t="n">
+      <c r="C24" s="90" t="n">
         <v>3582910082682</v>
       </c>
       <c r="D24" s="34" t="s">
@@ -15917,7 +15934,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="32" t="s">
@@ -15991,7 +16008,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="91" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="32" t="s">
@@ -16065,7 +16082,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="32" t="s">
@@ -16138,340 +16155,340 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="88" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="89" t="s">
+      <c r="B28" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="90" t="n">
+      <c r="C28" s="94" t="n">
         <v>8594739055421</v>
       </c>
-      <c r="D28" s="91" t="s">
+      <c r="D28" s="95" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="91" t="s">
+      <c r="E28" s="95" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="41" t="n">
         <v>1</v>
       </c>
-      <c r="G28" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" s="92" t="n">
+      <c r="G28" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="I28" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J28" s="92" t="n">
+      <c r="I28" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="K28" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="L28" s="93" t="n">
+      <c r="K28" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="M28" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="N28" s="93" t="n">
+      <c r="M28" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N28" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="O28" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="P28" s="92" t="n">
+      <c r="O28" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P28" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="Q28" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="R28" s="92" t="n">
+      <c r="Q28" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="R28" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="S28" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="T28" s="93" t="n">
+      <c r="S28" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="T28" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="U28" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="V28" s="93" t="n">
+      <c r="U28" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="V28" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="W28" s="92" t="n">
+      <c r="W28" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="X28" s="92" t="n">
+      <c r="X28" s="36" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="88" t="s">
+      <c r="A29" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="89" t="s">
+      <c r="B29" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="90" t="n">
+      <c r="C29" s="94" t="n">
         <v>3582910070252</v>
       </c>
-      <c r="D29" s="91" t="s">
+      <c r="D29" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="91" t="s">
+      <c r="E29" s="95" t="s">
         <v>73</v>
       </c>
       <c r="F29" s="41" t="n">
         <v>1</v>
       </c>
-      <c r="G29" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H29" s="92" t="n">
+      <c r="G29" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="I29" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J29" s="92" t="n">
+      <c r="I29" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="K29" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="L29" s="93" t="n">
+      <c r="K29" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="M29" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="N29" s="93" t="n">
+      <c r="M29" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N29" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="O29" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="P29" s="92" t="n">
+      <c r="O29" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P29" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="Q29" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="R29" s="92" t="n">
+      <c r="Q29" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="R29" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="S29" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="T29" s="93" t="n">
+      <c r="S29" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="T29" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="U29" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="V29" s="93" t="n">
+      <c r="U29" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="V29" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="W29" s="92" t="n">
+      <c r="W29" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="X29" s="92" t="n">
+      <c r="X29" s="36" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="89" t="s">
+      <c r="B30" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="90" t="n">
+      <c r="C30" s="94" t="n">
         <v>3582910077305</v>
       </c>
-      <c r="D30" s="91" t="s">
+      <c r="D30" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="91" t="s">
+      <c r="E30" s="95" t="s">
         <v>53</v>
       </c>
       <c r="F30" s="41" t="n">
         <v>1</v>
       </c>
-      <c r="G30" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H30" s="92" t="n">
+      <c r="G30" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="I30" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J30" s="92" t="n">
+      <c r="I30" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="K30" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="L30" s="93" t="n">
+      <c r="K30" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="M30" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="N30" s="93" t="n">
+      <c r="M30" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="O30" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="P30" s="92" t="n">
+      <c r="O30" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P30" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="Q30" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="R30" s="92" t="n">
+      <c r="Q30" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="R30" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="S30" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="T30" s="93" t="n">
+      <c r="S30" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="T30" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="U30" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="V30" s="93" t="n">
+      <c r="U30" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="V30" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="W30" s="92" t="n">
+      <c r="W30" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="X30" s="92" t="n">
+      <c r="X30" s="36" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="88" t="s">
+      <c r="A31" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="89" t="s">
+      <c r="B31" s="93" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="90" t="n">
+      <c r="C31" s="94" t="n">
         <v>3582910041870</v>
       </c>
-      <c r="D31" s="91" t="s">
+      <c r="D31" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="91" t="s">
+      <c r="E31" s="95" t="s">
         <v>81</v>
       </c>
       <c r="F31" s="41" t="n">
         <v>1</v>
       </c>
-      <c r="G31" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="H31" s="92" t="n">
+      <c r="G31" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="I31" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J31" s="92" t="n">
+      <c r="I31" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="K31" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="L31" s="93" t="n">
+      <c r="K31" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="M31" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="N31" s="93" t="n">
+      <c r="M31" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="O31" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="P31" s="92" t="n">
+      <c r="O31" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P31" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="Q31" s="92" t="n">
-        <v>1</v>
-      </c>
-      <c r="R31" s="92" t="n">
+      <c r="Q31" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="R31" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="S31" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="T31" s="93" t="n">
+      <c r="S31" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="T31" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="U31" s="93" t="n">
-        <v>1</v>
-      </c>
-      <c r="V31" s="93" t="n">
+      <c r="U31" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="V31" s="37" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="W31" s="92" t="n">
+      <c r="W31" s="36" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="X31" s="92" t="n">
+      <c r="X31" s="36" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H31"/>
+  <autoFilter ref="A2:G26"/>
   <mergeCells count="1">
     <mergeCell ref="G1:X1"/>
   </mergeCells>

</xml_diff>

<commit_message>
disable the block kpi
</commit_message>
<xml_diff>
--- a/Projects/SANOFIRU/Data/Template.xlsx
+++ b/Projects/SANOFIRU/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$31</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
@@ -44,6 +44,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$26</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
@@ -67,6 +68,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$12</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Primary_Brand_Blocking!$A$2:$H$12</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
@@ -77,30 +79,31 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$31</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$31</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$J$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$J$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$31</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$31</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$J$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$J$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$26</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -112,476 +115,470 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="139">
   <si>
-    <t xml:space="preserve">KPI Name</t>
+    <t>KPI Name</t>
   </si>
   <si>
-    <t xml:space="preserve">KPI Group</t>
+    <t>KPI Group</t>
   </si>
   <si>
-    <t xml:space="preserve">KPI Type</t>
+    <t>KPI Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Tested Group</t>
+    <t>Tested Group</t>
   </si>
   <si>
-    <t xml:space="preserve">Template Group</t>
+    <t>Template Group</t>
   </si>
   <si>
-    <t xml:space="preserve">Sheet</t>
+    <t>Sheet</t>
   </si>
   <si>
-    <t xml:space="preserve">SCORE</t>
+    <t>SCORE</t>
   </si>
   <si>
-    <t xml:space="preserve">POSM Availability Primary</t>
+    <t>POSM Availability Primary</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary Shelf</t>
+    <t>Primary Shelf</t>
   </si>
   <si>
-    <t xml:space="preserve">Product Availability Per SKU</t>
+    <t>Product Availability Per SKU</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary&amp;Secondary_POSM</t>
+    <t>Primary&amp;Secondary_POSM</t>
   </si>
   <si>
-    <t xml:space="preserve">numeric</t>
+    <t>numeric</t>
   </si>
   <si>
-    <t xml:space="preserve">Product Minimum Facings Primary</t>
+    <t>Product Minimum Facings Primary</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary&amp;Secondary_Facings</t>
+    <t>Primary&amp;Secondary_Facings</t>
   </si>
   <si>
-    <t xml:space="preserve">Blocked Together</t>
+    <t>POSM Availability Secondary</t>
   </si>
   <si>
-    <t xml:space="preserve">Blocked Together Per Brand</t>
+    <t>Secondary Shelf</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary_Brand_Blocking</t>
+    <t>Product Minimum Facings Secondary</t>
   </si>
   <si>
-    <t xml:space="preserve">POSM Availability Secondary</t>
+    <t>MSL Compliance</t>
   </si>
   <si>
-    <t xml:space="preserve">Secondary Shelf</t>
+    <t>MSL</t>
   </si>
   <si>
-    <t xml:space="preserve">Product Minimum Facings Secondary</t>
+    <t>Perfect Store</t>
   </si>
   <si>
-    <t xml:space="preserve">MSL Compliance</t>
+    <t>Primary Shelf Compliance</t>
   </si>
   <si>
-    <t xml:space="preserve">MSL</t>
+    <t>Secondary Shelf Compliance</t>
   </si>
   <si>
-    <t xml:space="preserve">Perfect Store</t>
+    <t>Perfect Store Compliance</t>
   </si>
   <si>
-    <t xml:space="preserve">Primary Shelf Compliance</t>
+    <t>Sum of KPIs in Group</t>
   </si>
   <si>
-    <t xml:space="preserve">Secondary Shelf Compliance</t>
+    <t>store type</t>
   </si>
   <si>
-    <t xml:space="preserve">Perfect Store Compliance</t>
+    <t>Product Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Sum of KPIs in Group</t>
+    <t>Product EAN Code</t>
   </si>
   <si>
-    <t xml:space="preserve">store type</t>
+    <t>Brand</t>
   </si>
   <si>
-    <t xml:space="preserve">Product Name</t>
+    <t>Category</t>
   </si>
   <si>
-    <t xml:space="preserve">Product EAN Code</t>
+    <t>Points</t>
   </si>
   <si>
-    <t xml:space="preserve">Brand</t>
+    <t>A w/ POSM w/ CD</t>
   </si>
   <si>
-    <t xml:space="preserve">Category</t>
+    <t>A w/ POSM w/o CD</t>
   </si>
   <si>
-    <t xml:space="preserve">Points</t>
+    <t>A w/o POSM w/ CD</t>
   </si>
   <si>
-    <t xml:space="preserve">A w/ POSM w/ CD</t>
+    <t>A w/o POSM w/o CD</t>
   </si>
   <si>
-    <t xml:space="preserve">A w/ POSM w/o CD</t>
+    <t>B-1 w/ POSM w/ CD</t>
   </si>
   <si>
-    <t xml:space="preserve">A w/o POSM w/ CD</t>
+    <t>B-1 w/ POSM w/o CD</t>
   </si>
   <si>
-    <t xml:space="preserve">A w/o POSM w/o CD</t>
+    <t>B-1 w/o POSM w/ CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-1 w/ POSM w/ CD</t>
+    <t>B-1 w/o POSM w/o CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-1 w/ POSM w/o CD</t>
+    <t>B-2 w/ POSM w/ CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-1 w/o POSM w/ CD</t>
+    <t>B-2 w/ POSM w/o CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-1 w/o POSM w/o CD</t>
+    <t>B-2 w/o POSM w/ CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-2 w/ POSM w/ CD</t>
+    <t>B-2 w/o POSM w/o CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-2 w/ POSM w/o CD</t>
+    <t>B-3 w/ POSM w/ CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-2 w/o POSM w/ CD</t>
+    <t>B-3 w/ POSM w/o CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-2 w/o POSM w/o CD</t>
+    <t>B-3 w/o POSM w/ CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-3 w/ POSM w/ CD</t>
+    <t>B-3 w/o POSM w/o CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-3 w/ POSM w/o CD</t>
+    <t>B-4 w/o POSM w/o CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-3 w/o POSM w/ CD</t>
+    <t>B-4 w/o POSM w/ CD</t>
   </si>
   <si>
-    <t xml:space="preserve">B-3 w/o POSM w/o CD</t>
+    <t>ESSENTIALE FORTE N 300MG CAP BL9X10</t>
   </si>
   <si>
-    <t xml:space="preserve">B-4 w/o POSM w/o CD</t>
+    <t>ESSENTIALE</t>
   </si>
   <si>
-    <t xml:space="preserve">B-4 w/o POSM w/ CD</t>
+    <t>Hepatoprotectors</t>
   </si>
   <si>
-    <t xml:space="preserve">ESSENTIALE FORTE N 300MG CAP BL9X10</t>
+    <t>ESSENTIALE FORTE N CAPS 300MG #30</t>
   </si>
   <si>
-    <t xml:space="preserve">ESSENTIALE</t>
+    <t>FESTAL DRAGEE 200MG #20</t>
   </si>
   <si>
-    <t xml:space="preserve">Hepatoprotectors</t>
+    <t>FESTAL</t>
   </si>
   <si>
-    <t xml:space="preserve">ESSENTIALE FORTE N CAPS 300MG #30</t>
+    <t>DH</t>
   </si>
   <si>
-    <t xml:space="preserve">FESTAL DRAGEE 200MG #20</t>
+    <t>FESTAL DRAGEE 200MG #40</t>
   </si>
   <si>
-    <t xml:space="preserve">FESTAL</t>
+    <t>FESTAL DRAGEE 200MG #100</t>
   </si>
   <si>
-    <t xml:space="preserve">DH</t>
+    <t>MAALOX TABS 400MG #20</t>
   </si>
   <si>
-    <t xml:space="preserve">FESTAL DRAGEE 200MG #40</t>
+    <t>MAALOX</t>
   </si>
   <si>
-    <t xml:space="preserve">FESTAL DRAGEE 200MG #100</t>
+    <t>MAALOX stick pack 4,3ml #6 red fruit taste</t>
   </si>
   <si>
-    <t xml:space="preserve">MAALOX TABS 400MG #20</t>
+    <t>GUTTALAX 300MG/40ML 30ML EEDRO BT1 M36RU</t>
   </si>
   <si>
-    <t xml:space="preserve">MAALOX</t>
+    <t>GUTTALAX</t>
   </si>
   <si>
-    <t xml:space="preserve">MAALOX stick pack 4,3ml #6 red fruit taste</t>
+    <t>LASOLVAN 300MG/40ML SOLIN BT1 M60 RU</t>
   </si>
   <si>
-    <t xml:space="preserve">GUTTALAX 300MG/40ML 30ML EEDRO BT1 M36RU</t>
+    <t>LASOLVAN</t>
   </si>
   <si>
-    <t xml:space="preserve">GUTTALAX</t>
+    <t>C&amp;C</t>
   </si>
   <si>
-    <t xml:space="preserve">LASOLVAN 300MG/40ML SOLIN BT1 M60 RU</t>
+    <t>LASOLVAN 15mg/5ml Syrup 100ml</t>
   </si>
   <si>
-    <t xml:space="preserve">LASOLVAN</t>
+    <t>LASOLVAN 30mg/5ml Syrup 100ml</t>
   </si>
   <si>
-    <t xml:space="preserve">C&amp;C</t>
+    <t>LASOLVAN MAX 75MG CAPCR BL1X10 M36 RU</t>
   </si>
   <si>
-    <t xml:space="preserve">LASOLVAN 15mg/5ml Syrup 100ml</t>
+    <t>MAGNE B6 TABS 48MG/5MG BLIST #50</t>
   </si>
   <si>
-    <t xml:space="preserve">LASOLVAN 30mg/5ml Syrup 100ml</t>
+    <t>MAGNE B6</t>
   </si>
   <si>
-    <t xml:space="preserve">LASOLVAN MAX 75MG CAPCR BL1X10 M36 RU</t>
+    <t>VMS</t>
   </si>
   <si>
-    <t xml:space="preserve">MAGNE B6 TABS 48MG/5MG BLIST #50</t>
+    <t>MAGNE B6 AMP 100MG/ 10MG/ 10ML #10</t>
   </si>
   <si>
-    <t xml:space="preserve">MAGNE B6</t>
+    <t>MAGNE B6 FORTE #30</t>
   </si>
   <si>
-    <t xml:space="preserve">VMS</t>
+    <t>D-SUN LEMON 20ML DROP</t>
   </si>
   <si>
-    <t xml:space="preserve">MAGNE B6 AMP 100MG/ 10MG/ 10ML #10</t>
+    <t>D-Sun</t>
   </si>
   <si>
-    <t xml:space="preserve">MAGNE B6 FORTE #30</t>
+    <t>D-SUN RASPBERRY 10ML DROP</t>
   </si>
   <si>
-    <t xml:space="preserve">D-SUN LEMON 20ML DROP</t>
+    <t>NO-SPA TABS 40MG #100</t>
   </si>
   <si>
-    <t xml:space="preserve">D-Sun</t>
+    <t>NO-SPA</t>
   </si>
   <si>
-    <t xml:space="preserve">D-SUN RASPBERRY 10ML DROP</t>
+    <t>Pain</t>
   </si>
   <si>
-    <t xml:space="preserve">NO-SPA TABS 40MG #100</t>
+    <t>NO-SPA 40mg #24</t>
   </si>
   <si>
-    <t xml:space="preserve">NO-SPA</t>
+    <t>NO-SPA TAB 40 MG (PUSH-TOP) #60</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain</t>
+    <t>NO-SPA FORTE 80MG TAB BL1X24 M36 RU</t>
   </si>
   <si>
-    <t xml:space="preserve">NO-SPA 40mg #24</t>
+    <t>FINALGON CREAM/35G 1/1,7+10,8MG/G RUS</t>
   </si>
   <si>
-    <t xml:space="preserve">NO-SPA TAB 40 MG (PUSH-TOP) #60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO-SPA FORTE 80MG TAB BL1X24 M36 RU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FINALGON CREAM/35G 1/1,7+10,8MG/G RUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+    <t>
 3582910082682 </t>
   </si>
   <si>
-    <t xml:space="preserve">FINALGON</t>
+    <t>FINALGON</t>
   </si>
   <si>
-    <t xml:space="preserve">FINALGON 25MG-4MG/G OINT TB1 M48 RU</t>
+    <t>FINALGON 25MG-4MG/G OINT TB1 M48 RU</t>
   </si>
   <si>
-    <t xml:space="preserve">Zodac GTT.20ML</t>
+    <t>Zodac GTT.20ML</t>
   </si>
   <si>
-    <t xml:space="preserve">ZODAC</t>
+    <t>ZODAC</t>
   </si>
   <si>
-    <t xml:space="preserve">Allergy</t>
+    <t>Allergy</t>
   </si>
   <si>
-    <t xml:space="preserve">Zodac TABS.FLM.30X10MG</t>
+    <t>Zodac TABS.FLM.30X10MG</t>
   </si>
   <si>
-    <t xml:space="preserve">SKUs</t>
+    <t>SKUs</t>
   </si>
   <si>
-    <t xml:space="preserve">Shelf Location Compliance</t>
+    <t>Shelf Location Compliance</t>
   </si>
   <si>
-    <t xml:space="preserve">Ignore Empty</t>
+    <t>Ignore Empty</t>
   </si>
   <si>
-    <t xml:space="preserve">ESSENTIALE FORTE N 300MG CAP BL9X10,
+    <t>Blocked Together</t>
+  </si>
+  <si>
+    <t>ESSENTIALE FORTE N 300MG CAP BL9X10,
 ESSENTIALE FORTE N CAPS 300MG #30</t>
   </si>
   <si>
-    <t xml:space="preserve">3582910078913,
+    <t>3582910078913,
 3582910077305</t>
   </si>
   <si>
-    <t xml:space="preserve">FESTAL DRAGEE 200MG #20,
+    <t>FESTAL DRAGEE 200MG #20,
 FESTAL DRAGEE 200MG #40,
 FESTAL DRAGEE 200MG #100</t>
   </si>
   <si>
-    <t xml:space="preserve">8901083060122,
+    <t>8901083060122,
 8901083060139,
 8901083060115</t>
   </si>
   <si>
-    <t xml:space="preserve">FESTAL DRAGEE 200MG #20,
+    <t>FESTAL DRAGEE 200MG #20,
 FESTAL DRAGEE 200MG #40</t>
   </si>
   <si>
-    <t xml:space="preserve">8901083060122,
+    <t>8901083060122,
 8901083060139</t>
   </si>
   <si>
-    <t xml:space="preserve">MAALOX TABS 400MG #20,
+    <t>MAALOX TABS 400MG #20,
 MAALOX stick pack 4,3ml #6 red fruit taste</t>
   </si>
   <si>
-    <t xml:space="preserve">3582910072218,
+    <t>3582910072218,
 3582910075660</t>
   </si>
   <si>
-    <t xml:space="preserve">Guttalax</t>
+    <t>Guttalax</t>
   </si>
   <si>
-    <t xml:space="preserve">LASOLVAN 300MG/40ML SOLIN BT1 M60 RU, 
+    <t>LASOLVAN 300MG/40ML SOLIN BT1 M60 RU, 
 LASOLVAN 15mg/5ml Syrup 100ml,
 LASOLVAN 30mg/5ml Syrup 100ml,
 LASOLVAN MAX 75MG CAPCR BL1X10 M36 RU,</t>
   </si>
   <si>
-    <t xml:space="preserve">9006968004082,
+    <t>9006968004082,
 9006968011882,
 9006968011479,
 9006968010793</t>
   </si>
   <si>
-    <t xml:space="preserve">LASOLVAN 300MG/40ML SOLIN BT1 M60 RU, 
+    <t>LASOLVAN 300MG/40ML SOLIN BT1 M60 RU, 
 LASOLVAN 15mg/5ml Syrup 100ml,
 LASOLVAN 30mg/5ml Syrup 100ml</t>
   </si>
   <si>
-    <t xml:space="preserve">9006968004082,
+    <t>9006968004082,
 9006968011882,
 9006968011479</t>
   </si>
   <si>
-    <t xml:space="preserve">MAGNE B6 TABS 48MG/5MG BLIST #50,
+    <t>MAGNE B6 TABS 48MG/5MG BLIST #50,
 MAGNE B6 AMP 100MG/ 10MG/ 10ML #10,
 MAGNE B6 FORTE #30</t>
   </si>
   <si>
-    <t xml:space="preserve">3582910070252,
+    <t>3582910070252,
 3582910026723,
 3582910071259</t>
   </si>
   <si>
-    <t xml:space="preserve">MAGNE B6 TABS 48MG/5MG BLIST #50,
+    <t>MAGNE B6 TABS 48MG/5MG BLIST #50,
 MAGNE B6 FORTE #30</t>
   </si>
   <si>
-    <t xml:space="preserve">3582910070252,
+    <t>3582910070252,
 3582910071259</t>
   </si>
   <si>
-    <t xml:space="preserve">D-SUN LEMON 20ML DROP,
+    <t>D-SUN LEMON 20ML DROP,
 D-SUN RASPBERRY 10ML DROP</t>
   </si>
   <si>
-    <t xml:space="preserve">7896070607590,
+    <t>7896070607590,
 7896070607606</t>
   </si>
   <si>
-    <t xml:space="preserve">NO-SPA TABS 40MG #100,
+    <t>NO-SPA TABS 40MG #100,
 NO-SPA 40mg #24,
 NO-SPA TAB 40 MG (PUSH-TOP) #60,
 NO-SPA FORTE 80MG TAB BL1X24 M36 RU</t>
   </si>
   <si>
-    <t xml:space="preserve">5997086103280,
+    <t>5997086103280,
 3582910060758,
 5997086105055,
 3582910062172</t>
   </si>
   <si>
-    <t xml:space="preserve">NO-SPA TABS 40MG #100,
+    <t>NO-SPA TABS 40MG #100,
 NO-SPA 40mg #24,
 NO-SPA TAB 40 MG (PUSH-TOP) #60</t>
   </si>
   <si>
-    <t xml:space="preserve">5997086103280,
+    <t>5997086103280,
 3582910060758,
 5997086105055</t>
   </si>
   <si>
-    <t xml:space="preserve">NO-SPA TABS 40MG #100,
+    <t>NO-SPA TABS 40MG #100,
 NO-SPA 40mg #24</t>
   </si>
   <si>
-    <t xml:space="preserve">5997086103280,
+    <t>5997086103280,
 3582910060758</t>
   </si>
   <si>
-    <t xml:space="preserve">FINALGON CREAM/35G 1/1,7+10,8MG/G RUS,
+    <t>FINALGON CREAM/35G 1/1,7+10,8MG/G RUS,
 FINALGON 25MG-4MG/G OINT TB1 M48 RU</t>
   </si>
   <si>
-    <t xml:space="preserve">3582910082682,
+    <t>3582910082682,
 9006968004532</t>
   </si>
   <si>
-    <t xml:space="preserve">Zodac TABS.FLM.30X10MG,
+    <t>Zodac TABS.FLM.30X10MG,
 Zodac GTT.20ML</t>
   </si>
   <si>
-    <t xml:space="preserve">8594739055421,
+    <t>8594739055421,
 8594739055209
 </t>
   </si>
   <si>
-    <t xml:space="preserve">8594739055209
+    <t>8594739055209
 </t>
   </si>
   <si>
-    <t xml:space="preserve">D-Sun primary POSM</t>
+    <t>D-Sun primary POSM</t>
   </si>
   <si>
-    <t xml:space="preserve">RU-ST-01</t>
+    <t>RU-ST-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Essentiale primary POSM</t>
+    <t>Essentiale primary POSM</t>
   </si>
   <si>
-    <t xml:space="preserve">RU-ST-02</t>
+    <t>RU-ST-02</t>
   </si>
   <si>
-    <t xml:space="preserve">Essentiale</t>
+    <t>Essentiale</t>
   </si>
   <si>
-    <t xml:space="preserve">Lasolvan primary POSM</t>
+    <t>Lasolvan primary POSM</t>
   </si>
   <si>
-    <t xml:space="preserve">RU-ST-03</t>
+    <t>RU-ST-03</t>
   </si>
   <si>
-    <t xml:space="preserve">Lasolvan</t>
+    <t>Lasolvan</t>
   </si>
   <si>
-    <t xml:space="preserve">Magne B6 primary POSM</t>
+    <t>Magne B6 primary POSM</t>
   </si>
   <si>
-    <t xml:space="preserve">RU-ST-04</t>
+    <t>RU-ST-04</t>
   </si>
   <si>
-    <t xml:space="preserve">Magne B6</t>
+    <t>Magne B6</t>
   </si>
   <si>
-    <t xml:space="preserve">No-spa primary POSM</t>
+    <t>No-spa primary POSM</t>
   </si>
   <si>
-    <t xml:space="preserve">RU-ST-05</t>
+    <t>RU-ST-05</t>
   </si>
   <si>
-    <t xml:space="preserve">No-Spa</t>
+    <t>No-Spa</t>
   </si>
   <si>
-    <t xml:space="preserve">No Spa 40 mg city pack #6</t>
+    <t>No Spa 40 mg city pack #6</t>
   </si>
 </sst>
 </file>
@@ -589,7 +586,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0"/>
@@ -1035,7 +1032,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="93">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1296,18 +1293,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1521,15 +1506,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1001880</xdr:colOff>
+      <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>274320</xdr:rowOff>
+      <xdr:rowOff>265320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1002240</xdr:colOff>
+      <xdr:colOff>1029240</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>274680</xdr:rowOff>
+      <xdr:rowOff>265680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1542,7 +1527,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4180680" y="1474920"/>
+          <a:off x="4229280" y="1465920"/>
           <a:ext cx="360" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1558,15 +1543,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>915120</xdr:colOff>
+      <xdr:colOff>942120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>261720</xdr:rowOff>
+      <xdr:rowOff>252720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>915480</xdr:colOff>
+      <xdr:colOff>942480</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>377640</xdr:rowOff>
+      <xdr:rowOff>368280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1579,8 +1564,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4093920" y="1462320"/>
-          <a:ext cx="360" cy="115920"/>
+          <a:off x="4142520" y="1453320"/>
+          <a:ext cx="360" cy="115560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1600,15 +1585,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1999800</xdr:colOff>
+      <xdr:colOff>2026800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>284400</xdr:rowOff>
+      <xdr:rowOff>275400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2000520</xdr:colOff>
+      <xdr:colOff>2027160</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>473760</xdr:rowOff>
+      <xdr:rowOff>464400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1621,8 +1606,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4231080" y="901440"/>
-          <a:ext cx="720" cy="189360"/>
+          <a:off x="4274640" y="892440"/>
+          <a:ext cx="360" cy="189000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1648,19 +1633,19 @@
   </sheetPr>
   <dimension ref="A1:G65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3441295546559"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8947368421053"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0931174089069"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.4412955465587"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.9473684210526"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.7773279352227"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.8178137651822"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,22 +1713,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>8</v>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>11</v>
@@ -1751,135 +1736,115 @@
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="8" t="s">
+    <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="13"/>
+      <c r="D7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="15"/>
       <c r="F7" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>9</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C8" s="11"/>
       <c r="D8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="B9" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="11"/>
       <c r="G9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="13"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="20" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="20" t="s">
-        <v>11</v>
-      </c>
-    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1906,15 +1871,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.7611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0364372469636"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.834008097166"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7732793522267"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.8461538461538"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.1336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9230769230769"/>
     <col collapsed="false" hidden="true" max="6" min="6" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.2267206477733"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1925,7 +1890,7 @@
       <c r="E1" s="24"/>
       <c r="F1" s="25"/>
       <c r="G1" s="26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H1" s="26"/>
       <c r="I1" s="26"/>
@@ -1950,90 +1915,90 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="F2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="G2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="H2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="I2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="J2" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="N2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="R2" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="S2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="T2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="U2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="30" t="s">
+      <c r="V2" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="30" t="s">
+      <c r="W2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="30" t="s">
+      <c r="X2" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="30" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C3" s="33" t="n">
         <v>3582910078913</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F3" s="35"/>
       <c r="G3" s="36" t="n">
@@ -2093,19 +2058,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" s="33" t="n">
         <v>3582910077305</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F4" s="38"/>
       <c r="G4" s="36" t="n">
@@ -2165,19 +2130,19 @@
     </row>
     <row r="5" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C5" s="33" t="n">
         <v>8901083060122</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F5" s="38"/>
       <c r="G5" s="36" t="n">
@@ -2239,19 +2204,19 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C6" s="33" t="n">
         <v>8901083060139</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="36" t="n">
@@ -2311,19 +2276,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" s="33" t="n">
         <v>8901083060115</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F7" s="40"/>
       <c r="G7" s="36" t="n">
@@ -2383,19 +2348,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C8" s="33" t="n">
         <v>3582910072218</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F8" s="41"/>
       <c r="G8" s="36" t="n">
@@ -2455,19 +2420,19 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C9" s="33" t="n">
         <v>3582910075660</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F9" s="41"/>
       <c r="G9" s="36" t="n">
@@ -2527,19 +2492,19 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C10" s="33" t="n">
         <v>9006968001890</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F10" s="41"/>
       <c r="G10" s="36" t="n">
@@ -2599,19 +2564,19 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C11" s="42" t="n">
         <v>9006968004082</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F11" s="44"/>
       <c r="G11" s="45" t="n">
@@ -2671,19 +2636,19 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C12" s="42" t="n">
         <v>9006968011882</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F12" s="44"/>
       <c r="G12" s="45" t="n">
@@ -2743,19 +2708,19 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C13" s="42" t="n">
         <v>9006968011479</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F13" s="44"/>
       <c r="G13" s="45" t="n">
@@ -2815,19 +2780,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C14" s="42" t="n">
         <v>9006968010793</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E14" s="43" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F14" s="44"/>
       <c r="G14" s="45" t="n">
@@ -2887,19 +2852,19 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C15" s="33" t="n">
         <v>3582910070252</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F15" s="47"/>
       <c r="G15" s="36" t="n">
@@ -2959,19 +2924,19 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C16" s="33" t="n">
         <v>3582910026723</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F16" s="47"/>
       <c r="G16" s="36" t="n">
@@ -3031,19 +2996,19 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C17" s="33" t="n">
         <v>3582910071259</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F17" s="47"/>
       <c r="G17" s="36" t="n">
@@ -3103,19 +3068,19 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C18" s="33" t="n">
         <v>7896070607590</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F18" s="47"/>
       <c r="G18" s="36" t="n">
@@ -3175,19 +3140,19 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C19" s="33" t="n">
         <v>7896070607606</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19" s="47"/>
       <c r="G19" s="36" t="n">
@@ -3247,19 +3212,19 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C20" s="33" t="n">
         <v>5997086103280</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F20" s="47"/>
       <c r="G20" s="36" t="n">
@@ -3319,19 +3284,19 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C21" s="33" t="n">
         <v>3582910060758</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F21" s="47"/>
       <c r="G21" s="36" t="n">
@@ -3391,19 +3356,19 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C22" s="33" t="n">
         <v>5997086105055</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F22" s="47"/>
       <c r="G22" s="36" t="n">
@@ -3463,19 +3428,19 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C23" s="33" t="n">
         <v>3582910062172</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F23" s="47"/>
       <c r="G23" s="36" t="n">
@@ -3535,19 +3500,19 @@
     </row>
     <row r="24" customFormat="false" ht="22.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F24" s="47"/>
       <c r="G24" s="36" t="n">
@@ -3607,19 +3572,19 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C25" s="33" t="n">
         <v>9006968004532</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F25" s="47"/>
       <c r="G25" s="36" t="n">
@@ -3679,19 +3644,19 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C26" s="33" t="n">
         <v>8594739055209</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F26" s="47"/>
       <c r="G26" s="36" t="n">
@@ -3751,19 +3716,19 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C27" s="33" t="n">
         <v>8594739055421</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F27" s="47"/>
       <c r="G27" s="36" t="n">
@@ -3856,13 +3821,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0364372469636"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.82995951417"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.7611336032389"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8947368421053"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.97570850202429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.1336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3872,7 +3837,7 @@
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
       <c r="F1" s="26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
@@ -3897,75 +3862,75 @@
         <v>0</v>
       </c>
       <c r="B2" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="G2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="29" t="s">
+      <c r="H2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="J2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="N2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="R2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="S2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="T2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="30" t="s">
+      <c r="U2" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="30" t="s">
+      <c r="V2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="T2" s="30" t="s">
+      <c r="W2" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="U2" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -3992,7 +3957,7 @@
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B4" s="50"/>
       <c r="C4" s="50"/>
@@ -4019,7 +3984,7 @@
     </row>
     <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -4046,7 +4011,7 @@
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
@@ -4073,7 +4038,7 @@
     </row>
     <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50"/>
@@ -4100,7 +4065,7 @@
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="50"/>
@@ -4127,7 +4092,7 @@
     </row>
     <row r="9" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
@@ -4154,7 +4119,7 @@
     </row>
     <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
@@ -4181,7 +4146,7 @@
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
@@ -4208,7 +4173,7 @@
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
@@ -4257,22 +4222,22 @@
   </sheetPr>
   <dimension ref="A1:AMH21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R27" activeCellId="0" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="14.2024291497976"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="10.5263157894737"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="40.7611336032389"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="23.0161943319838"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="16.7732793522267"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="52" width="6.24291497975709"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="52" width="6.12145748987854"/>
-    <col collapsed="false" hidden="false" max="1022" min="9" style="52" width="9.30364372469636"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="41.1336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="52" width="6.21457489878543"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="52" width="6.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1022" min="9" style="52" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4283,7 +4248,7 @@
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H1" s="25"/>
       <c r="I1" s="25"/>
@@ -5306,73 +5271,73 @@
         <v>0</v>
       </c>
       <c r="B2" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="H2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="29" t="s">
+      <c r="I2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="N2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="R2" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="S2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="T2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="U2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="30" t="s">
+      <c r="V2" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="30" t="s">
+      <c r="W2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="30" t="s">
+      <c r="X2" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="30" t="s">
-        <v>50</v>
       </c>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
@@ -6375,19 +6340,19 @@
     </row>
     <row r="3" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F3" s="58" t="n">
         <v>1</v>
@@ -7447,19 +7412,19 @@
     </row>
     <row r="4" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D4" s="56" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E4" s="57" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F4" s="58" t="n">
         <v>1</v>
@@ -8519,19 +8484,19 @@
     </row>
     <row r="5" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E5" s="57" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F5" s="58" t="n">
         <v>1</v>
@@ -8593,19 +8558,19 @@
     </row>
     <row r="6" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E6" s="57" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F6" s="58" t="n">
         <v>1</v>
@@ -8667,16 +8632,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D7" s="61" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E7" s="57" t="n">
         <v>3582910075660</v>
@@ -8741,16 +8706,16 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D8" s="61" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E8" s="57" t="n">
         <v>9006968001890</v>
@@ -8815,19 +8780,19 @@
     </row>
     <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D9" s="56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E9" s="57" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F9" s="58" t="n">
         <v>1</v>
@@ -8889,19 +8854,19 @@
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D10" s="56" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F10" s="58" t="n">
         <v>1</v>
@@ -8963,16 +8928,16 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D11" s="56" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E11" s="57" t="n">
         <v>9006968011882</v>
@@ -9037,19 +9002,19 @@
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D12" s="56" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F12" s="58" t="n">
         <v>1</v>
@@ -9111,19 +9076,19 @@
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F13" s="58" t="n">
         <v>1</v>
@@ -9185,19 +9150,19 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="62" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D14" s="56" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F14" s="58" t="n">
         <v>1</v>
@@ -9259,19 +9224,19 @@
     </row>
     <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D15" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F15" s="58" t="n">
         <v>1</v>
@@ -9333,19 +9298,19 @@
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D16" s="56" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F16" s="58" t="n">
         <v>1</v>
@@ -9407,19 +9372,19 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D17" s="56" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E17" s="57" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F17" s="58" t="n">
         <v>1</v>
@@ -9481,19 +9446,19 @@
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D18" s="56" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E18" s="57" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F18" s="58" t="n">
         <v>1</v>
@@ -9555,16 +9520,16 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="55" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D19" s="56" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E19" s="57" t="n">
         <v>9006968004532</v>
@@ -9629,149 +9594,149 @@
     </row>
     <row r="20" customFormat="false" ht="27.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="62" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D20" s="56" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E20" s="57" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F20" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="G20" s="65" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="I20" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="J20" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="K20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="R20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="S20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="T20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="U20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="V20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="W20" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="X20" s="67" t="n">
+      <c r="G20" s="59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" s="60" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="68" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="69" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" s="70" t="s">
-        <v>125</v>
-      </c>
-      <c r="F21" s="71" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="L21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="M21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="N21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="O21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="P21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="R21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="S21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="T21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="U21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="V21" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="W21" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="X21" s="74" t="n">
+        <v>93</v>
+      </c>
+      <c r="B21" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="P21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="R21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="T21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="U21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="V21" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="W21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" s="71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9804,15 +9769,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="25.0931174089069"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="26.080971659919"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="60.3522267206478"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="10.6558704453441"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="6.24291497975709"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="52" width="6.12145748987854"/>
-    <col collapsed="false" hidden="false" max="1022" min="8" style="52" width="9.30364372469636"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="60.8421052631579"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="6.21457489878543"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="52" width="6.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1022" min="8" style="52" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9822,7 +9787,7 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
       <c r="F1" s="25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
@@ -9847,326 +9812,326 @@
         <v>0</v>
       </c>
       <c r="B2" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="48" t="s">
+      <c r="F2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="G2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="H2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="J2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="N2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="R2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="S2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="T2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="30" t="s">
+      <c r="U2" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="30" t="s">
+      <c r="V2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="T2" s="30" t="s">
+      <c r="W2" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="U2" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="77" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="78" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" s="79"/>
-      <c r="U3" s="79"/>
-      <c r="V3" s="80"/>
-      <c r="W3" s="80"/>
+      <c r="B3" s="73" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="77"/>
+      <c r="W3" s="77"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="77" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="78" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="81" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="81" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" s="82" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="80"/>
+      <c r="E4" s="79" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="77"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="73" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="79" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" s="79" t="s">
-        <v>133</v>
-      </c>
-      <c r="E5" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="P5" s="79"/>
-      <c r="Q5" s="79"/>
-      <c r="R5" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="S5" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" s="79"/>
-      <c r="U5" s="79"/>
-      <c r="V5" s="76"/>
-      <c r="W5" s="76"/>
+      <c r="E5" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="76"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="73"/>
+      <c r="W5" s="73"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="79" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="79" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" s="79" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="O6" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="S6" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="T6" s="79"/>
-      <c r="U6" s="79"/>
-      <c r="V6" s="76"/>
-      <c r="W6" s="76"/>
+      <c r="E6" s="76" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="76"/>
+      <c r="R6" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="76"/>
+      <c r="U6" s="76"/>
+      <c r="V6" s="73"/>
+      <c r="W6" s="73"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="79" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="79" t="s">
-        <v>139</v>
-      </c>
-      <c r="E7" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="79"/>
-      <c r="R7" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="S7" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" s="79"/>
-      <c r="U7" s="79"/>
-      <c r="V7" s="76"/>
-      <c r="W7" s="76"/>
+      <c r="E7" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="P7" s="76"/>
+      <c r="Q7" s="76"/>
+      <c r="R7" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" s="76"/>
+      <c r="U7" s="76"/>
+      <c r="V7" s="73"/>
+      <c r="W7" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10197,16 +10162,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="32.4412955465587"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="34.8906882591093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="14.3238866396761"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="10.5263157894737"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="52" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="52" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="10.5263157894737"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="52" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="52" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="52" width="6.12145748987854"/>
-    <col collapsed="false" hidden="false" max="1022" min="9" style="52" width="9.30364372469636"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="52" width="6.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1022" min="9" style="52" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10216,26 +10181,26 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
       <c r="F1" s="25"/>
-      <c r="G1" s="84" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
+      <c r="G1" s="81" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="81"/>
+      <c r="W1" s="81"/>
+      <c r="X1" s="81"/>
       <c r="Y1" s="0"/>
       <c r="Z1" s="0"/>
       <c r="AA1" s="0"/>
@@ -11236,77 +11201,77 @@
       <c r="AMH1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="48.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="86" t="s">
+      <c r="A2" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="83" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="F2" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="G2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="86" t="s">
+      <c r="H2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="I2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="J2" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="N2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="R2" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="S2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="T2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="U2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="30" t="s">
+      <c r="V2" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="30" t="s">
+      <c r="W2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="30" t="s">
+      <c r="X2" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="30" t="s">
-        <v>50</v>
       </c>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
@@ -12308,20 +12273,20 @@
       <c r="AMH2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C3" s="33" t="n">
         <v>3582910078913</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F3" s="41" t="n">
         <v>1</v>
@@ -13380,20 +13345,20 @@
       <c r="AMH3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" s="33" t="n">
         <v>3582910077305</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F4" s="41" t="n">
         <v>1</v>
@@ -14452,20 +14417,20 @@
       <c r="AMH4" s="0"/>
     </row>
     <row r="5" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C5" s="33" t="n">
         <v>8901083060122</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F5" s="41" t="n">
         <v>1</v>
@@ -14528,20 +14493,20 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C6" s="33" t="n">
         <v>8901083060139</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F6" s="41" t="n">
         <v>1</v>
@@ -14602,20 +14567,20 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" s="33" t="n">
         <v>8901083060115</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F7" s="41" t="n">
         <v>1</v>
@@ -14676,20 +14641,20 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C8" s="33" t="n">
         <v>3582910072218</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F8" s="41" t="n">
         <v>1</v>
@@ -14750,20 +14715,20 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C9" s="33" t="n">
         <v>3582910075660</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F9" s="41" t="n">
         <v>1</v>
@@ -14824,20 +14789,20 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="85" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C10" s="33" t="n">
         <v>9006968001890</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F10" s="41" t="n">
         <v>1</v>
@@ -14898,20 +14863,20 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C11" s="33" t="n">
         <v>9006968004082</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F11" s="41" t="n">
         <v>1</v>
@@ -14972,20 +14937,20 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C12" s="33" t="n">
         <v>9006968011882</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F12" s="41" t="n">
         <v>1</v>
@@ -15046,20 +15011,20 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C13" s="33" t="n">
         <v>9006968011479</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F13" s="41" t="n">
         <v>1</v>
@@ -15120,20 +15085,20 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C14" s="33" t="n">
         <v>9006968010793</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F14" s="41" t="n">
         <v>1</v>
@@ -15194,20 +15159,20 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="88" t="s">
+      <c r="A15" s="85" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C15" s="33" t="n">
         <v>3582910070252</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F15" s="41" t="n">
         <v>1</v>
@@ -15268,20 +15233,20 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="85" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C16" s="33" t="n">
         <v>3582910026723</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F16" s="41" t="n">
         <v>1</v>
@@ -15342,20 +15307,20 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="85" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C17" s="33" t="n">
         <v>3582910071259</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F17" s="41" t="n">
         <v>1</v>
@@ -15416,20 +15381,20 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C18" s="33" t="n">
         <v>7896070607590</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F18" s="41" t="n">
         <v>1</v>
@@ -15490,20 +15455,20 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="75" t="s">
+      <c r="A19" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C19" s="33" t="n">
         <v>7896070607606</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19" s="41" t="n">
         <v>1</v>
@@ -15564,20 +15529,20 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C20" s="33" t="n">
         <v>5997086103280</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F20" s="41" t="n">
         <v>1</v>
@@ -15638,20 +15603,20 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C21" s="33" t="n">
         <v>3582910060758</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F21" s="41" t="n">
         <v>1</v>
@@ -15712,20 +15677,20 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C22" s="33" t="n">
         <v>5997086105055</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F22" s="41" t="n">
         <v>1</v>
@@ -15786,20 +15751,20 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="89" t="n">
+        <v>81</v>
+      </c>
+      <c r="C23" s="86" t="n">
         <v>3582910062172</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F23" s="41" t="n">
         <v>1</v>
@@ -15860,20 +15825,20 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="90" t="n">
+        <v>82</v>
+      </c>
+      <c r="C24" s="87" t="n">
         <v>3582910082682</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F24" s="41" t="n">
         <v>1</v>
@@ -15934,20 +15899,20 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="75" t="s">
+      <c r="A25" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C25" s="33" t="n">
         <v>9006968004532</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F25" s="41" t="n">
         <v>1</v>
@@ -16008,20 +15973,20 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="88" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C26" s="33" t="n">
         <v>8594739055209</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F26" s="41" t="n">
         <v>1</v>
@@ -16082,20 +16047,20 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C27" s="33" t="n">
         <v>8594739055421</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F27" s="41" t="n">
         <v>1</v>
@@ -16156,20 +16121,20 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="92" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="93" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="94" t="n">
+      <c r="A28" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="90" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="91" t="n">
         <v>8594739055421</v>
       </c>
-      <c r="D28" s="95" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="95" t="s">
-        <v>91</v>
+      <c r="D28" s="92" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="92" t="s">
+        <v>88</v>
       </c>
       <c r="F28" s="41" t="n">
         <v>1</v>
@@ -16239,20 +16204,20 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="92" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="93" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="94" t="n">
+      <c r="A29" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="90" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="91" t="n">
         <v>3582910070252</v>
       </c>
-      <c r="D29" s="95" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" s="95" t="s">
-        <v>73</v>
+      <c r="D29" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="92" t="s">
+        <v>70</v>
       </c>
       <c r="F29" s="41" t="n">
         <v>1</v>
@@ -16322,20 +16287,20 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="92" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="93" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="94" t="n">
+      <c r="A30" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="90" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="91" t="n">
         <v>3582910077305</v>
       </c>
-      <c r="D30" s="95" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="95" t="s">
-        <v>53</v>
+      <c r="D30" s="92" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="92" t="s">
+        <v>50</v>
       </c>
       <c r="F30" s="41" t="n">
         <v>1</v>
@@ -16405,20 +16370,20 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="92" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="93" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="94" t="n">
+      <c r="A31" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="90" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="91" t="n">
         <v>3582910041870</v>
       </c>
-      <c r="D31" s="95" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="95" t="s">
-        <v>81</v>
+      <c r="D31" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="92" t="s">
+        <v>78</v>
       </c>
       <c r="F31" s="41" t="n">
         <v>1</v>
@@ -16488,7 +16453,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G26"/>
+  <autoFilter ref="A2:H31"/>
   <mergeCells count="1">
     <mergeCell ref="G1:X1"/>
   </mergeCells>

</xml_diff>